<commit_message>
more progress. need to check why e gets corrupted, also check MbyM_std with inversion
</commit_message>
<xml_diff>
--- a/visualization.xlsx
+++ b/visualization.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>sample</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>prediction</t>
-  </si>
-  <si>
-    <t>target</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
   <dimension ref="A2:BI23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AX11" sqref="AX11:BI11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +546,7 @@
   <sheetData>
     <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>

</xml_diff>